<commit_message>
updated Excel file with final plastic weights
</commit_message>
<xml_diff>
--- a/Data/RawData/meta_plastic.xlsx
+++ b/Data/RawData/meta_plastic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mountallison-my.sharepoint.com/personal/hrmactavish_mta_ca/Documents/24_micro/plastic_degrade/Data/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{A1FBDEB2-F410-46DA-9CED-5A2D4F84944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C102733B-E9A3-42CE-8ED9-36D1C7AE73AE}"/>
+  <xr:revisionPtr revIDLastSave="328" documentId="8_{A1FBDEB2-F410-46DA-9CED-5A2D4F84944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16285B4-3160-4031-84C5-4399A677A6BB}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="19800" windowHeight="9720" xr2:uid="{5CFE263B-8B26-445F-ABCD-D4D78ECA3A9E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="DataDictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,11 +37,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>BioReactor</t>
+  </si>
+  <si>
+    <t>Culture_Present</t>
+  </si>
+  <si>
+    <t>Nutrient_Present</t>
+  </si>
+  <si>
+    <t>Plastic_Present</t>
+  </si>
+  <si>
+    <t>Temperature_C</t>
+  </si>
+  <si>
+    <t>Initial_Plastic_Weight_mg</t>
+  </si>
+  <si>
+    <t>Culture_Volume_mL</t>
+  </si>
+  <si>
+    <t>Nutrient_Volume_mL</t>
+  </si>
+  <si>
+    <t>Final_Plastic_Weight_mg</t>
+  </si>
+  <si>
+    <t>Control_or_Replicate</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>ExpStartDate</t>
+  </si>
+  <si>
+    <t>ExpEndDate</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
   <si>
     <t>CAPL001</t>
   </si>
   <si>
+    <t>Mix004</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>MCMIX004</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
     <t>CAPL002</t>
   </si>
   <si>
@@ -57,6 +123,12 @@
     <t>CAPL006</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
     <t>CAPL007</t>
   </si>
   <si>
@@ -66,6 +138,12 @@
     <t>CAPL009</t>
   </si>
   <si>
+    <t>Mix006</t>
+  </si>
+  <si>
+    <t>MCMIX006</t>
+  </si>
+  <si>
     <t>CAPL010</t>
   </si>
   <si>
@@ -87,179 +165,101 @@
     <t>CAPL016</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>BioReactor</t>
-  </si>
-  <si>
-    <t>Mix004</t>
-  </si>
-  <si>
-    <t>Mix006</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Code to identify the tube by</t>
   </si>
   <si>
-    <t>Temperature_C</t>
-  </si>
-  <si>
-    <t>Culture_Present</t>
-  </si>
-  <si>
-    <t>Nutrient_Present</t>
-  </si>
-  <si>
-    <t>Plastic_Present</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Which BioReactor the tube is in</t>
   </si>
   <si>
     <t>Was culture added to the tube</t>
   </si>
   <si>
+    <t>1 = Yes, 0 =No</t>
+  </si>
+  <si>
     <t>Was nutrient added to the tube</t>
   </si>
   <si>
+    <t>2 = Yes, 0 =No</t>
+  </si>
+  <si>
     <t>Was plastic added to the tube</t>
   </si>
   <si>
+    <t>3 = Yes, 0 =No</t>
+  </si>
+  <si>
     <t>What temperature the BioReactor is set to</t>
   </si>
   <si>
     <t>degrees C</t>
   </si>
   <si>
-    <t>1 = Yes, 0 =No</t>
-  </si>
-  <si>
-    <t>2 = Yes, 0 =No</t>
-  </si>
-  <si>
-    <t>3 = Yes, 0 =No</t>
-  </si>
-  <si>
-    <t>Initial_Plastic_Weight_mg</t>
-  </si>
-  <si>
     <t>The weight of the plastic before put in the tube</t>
   </si>
   <si>
     <t>mg</t>
   </si>
   <si>
-    <t>Culture_Volume_mL</t>
-  </si>
-  <si>
-    <t>Nutrient_Volume_mL</t>
-  </si>
-  <si>
-    <t>Final_Plastic_Weight_mg</t>
-  </si>
-  <si>
     <t>Initial volume of the culture added to the tube</t>
   </si>
   <si>
+    <t>mL</t>
+  </si>
+  <si>
     <t>Initial volume of the nutient added to the tube</t>
   </si>
   <si>
     <t>Final weight of the plastic after 6 week period</t>
   </si>
   <si>
-    <t>mL</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Control_or_Replicate</t>
-  </si>
-  <si>
-    <t>Replicate</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
     <t>Is tube a  control or a replicate</t>
   </si>
   <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>Tube</t>
-  </si>
-  <si>
-    <t>WL</t>
-  </si>
-  <si>
-    <t>WW</t>
-  </si>
-  <si>
-    <t>MCMIX004</t>
-  </si>
-  <si>
-    <t>MCMIX006</t>
-  </si>
-  <si>
-    <t>Plastic</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>ExpStartDate</t>
-  </si>
-  <si>
-    <t>ExpEndDate</t>
+    <t>BioReactor identifier associated with the BioReactor data</t>
+  </si>
+  <si>
+    <t>Tube number associated with the BioReactor data</t>
+  </si>
+  <si>
+    <t>Wave Length (light colour)</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Clarify what WW means</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date BioReacter was started </t>
+  </si>
+  <si>
+    <t>YMD</t>
   </si>
   <si>
     <t>Date BioReacter was stopped and data was exported</t>
   </si>
   <si>
-    <t xml:space="preserve">Date BioReacter was started </t>
-  </si>
-  <si>
-    <t>YMD</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Clarify what WW means</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Tube number associated with the BioReactor data</t>
-  </si>
-  <si>
-    <t>BioReactor identifier associated with the BioReactor data</t>
-  </si>
-  <si>
     <t>Project name assocaited with BioReactor data</t>
-  </si>
-  <si>
-    <t>Wave Length (light colour)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,81 +673,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35ADBD4-5335-48F8-A626-2D48166F0073}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P17"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="13.9">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
@@ -773,18 +773,20 @@
       <c r="I2" s="1">
         <v>0.4</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>44.366999999999997</v>
+      </c>
       <c r="K2" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O2">
         <v>20240927</v>
@@ -793,12 +795,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -824,18 +826,20 @@
       <c r="I3" s="1">
         <v>0.4</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>41.216000000000001</v>
+      </c>
       <c r="K3" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O3">
         <v>20240927</v>
@@ -844,12 +848,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
@@ -875,18 +879,20 @@
       <c r="I4" s="1">
         <v>0.4</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>43.107999999999997</v>
+      </c>
       <c r="K4" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O4">
         <v>20240927</v>
@@ -895,12 +901,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -926,18 +932,20 @@
       <c r="I5" s="1">
         <v>0.4</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>38.700000000000003</v>
+      </c>
       <c r="K5" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O5">
         <v>20240927</v>
@@ -946,12 +954,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -977,18 +985,20 @@
       <c r="I6" s="1">
         <v>0.4</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>32.731999999999999</v>
+      </c>
       <c r="K6" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O6">
         <v>20240927</v>
@@ -997,12 +1007,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -1020,7 +1030,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1">
         <v>80</v>
@@ -1028,18 +1038,20 @@
       <c r="I7" s="1">
         <v>0.4</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="K7" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O7">
         <v>20240927</v>
@@ -1048,12 +1060,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -1079,18 +1091,20 @@
       <c r="I8" s="1">
         <v>0.4</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <v>31.373999999999999</v>
+      </c>
       <c r="K8" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O8">
         <v>20240927</v>
@@ -1099,12 +1113,12 @@
         <v>20241029100000</v>
       </c>
       <c r="Q8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -1130,18 +1144,20 @@
       <c r="I9" s="1">
         <v>0.4</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <v>38.19</v>
+      </c>
       <c r="K9" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O9">
         <v>20240927</v>
@@ -1150,15 +1166,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -1181,18 +1197,20 @@
       <c r="I10" s="1">
         <v>0.4</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>38.9</v>
+      </c>
       <c r="K10" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O10">
         <v>20240927</v>
@@ -1201,15 +1219,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -1232,18 +1250,20 @@
       <c r="I11" s="1">
         <v>0.4</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <v>35.029000000000003</v>
+      </c>
       <c r="K11" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O11">
         <v>20240927</v>
@@ -1252,15 +1272,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1275,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H12" s="1">
         <v>80</v>
@@ -1283,18 +1303,20 @@
       <c r="I12" s="1">
         <v>0.4</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="K12" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M12">
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O12">
         <v>20240927</v>
@@ -1303,15 +1325,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -1334,18 +1356,20 @@
       <c r="I13" s="1">
         <v>0.4</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>31.009</v>
+      </c>
       <c r="K13" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M13">
         <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O13">
         <v>20240927</v>
@@ -1354,15 +1378,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1385,18 +1409,20 @@
       <c r="I14" s="1">
         <v>0.4</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>29.66</v>
+      </c>
       <c r="K14" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M14">
         <v>5</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O14">
         <v>20240927</v>
@@ -1405,15 +1431,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1436,18 +1462,20 @@
       <c r="I15" s="1">
         <v>0.4</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <v>44.78</v>
+      </c>
       <c r="K15" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M15">
         <v>6</v>
       </c>
       <c r="N15" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O15">
         <v>20240927</v>
@@ -1456,15 +1484,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1487,18 +1515,20 @@
       <c r="I16" s="1">
         <v>0.4</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>35.579000000000001</v>
+      </c>
       <c r="K16" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M16">
         <v>7</v>
       </c>
       <c r="N16" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O16">
         <v>20240927</v>
@@ -1507,15 +1537,15 @@
         <v>20241029100000</v>
       </c>
       <c r="Q16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1538,18 +1568,20 @@
       <c r="I17" s="1">
         <v>0.4</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>41.765000000000001</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="L17" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M17">
         <v>8</v>
       </c>
       <c r="N17" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="O17">
         <v>20240927</v>
@@ -1558,7 +1590,7 @@
         <v>20241029100000</v>
       </c>
       <c r="Q17" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1575,218 +1607,218 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the RFU data (tried last week and was having WiFi driver issues)
</commit_message>
<xml_diff>
--- a/Data/RawData/meta_plastic.xlsx
+++ b/Data/RawData/meta_plastic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mountallison-my.sharepoint.com/personal/hrmactavish_mta_ca/Documents/24_micro/plastic_degrade/Data/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="328" documentId="8_{A1FBDEB2-F410-46DA-9CED-5A2D4F84944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16285B4-3160-4031-84C5-4399A677A6BB}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{A1FBDEB2-F410-46DA-9CED-5A2D4F84944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BD17090-D293-4516-9299-015A97EEE03A}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="19800" windowHeight="9720" xr2:uid="{5CFE263B-8B26-445F-ABCD-D4D78ECA3A9E}"/>
+    <workbookView xWindow="11376" yWindow="204" windowWidth="11184" windowHeight="11556" xr2:uid="{5CFE263B-8B26-445F-ABCD-D4D78ECA3A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="77">
   <si>
     <t>Identifier</t>
   </si>
@@ -253,13 +253,28 @@
   </si>
   <si>
     <t>Project name assocaited with BioReactor data</t>
+  </si>
+  <si>
+    <t>Wall_Growth_RFU</t>
+  </si>
+  <si>
+    <t>Suspension_RFU</t>
+  </si>
+  <si>
+    <t>RFU</t>
+  </si>
+  <si>
+    <t>Chlorophyll a reading from growth on the tube wall</t>
+  </si>
+  <si>
+    <t>Chlorophyll a reading after growth was suspended</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,28 +686,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35ADBD4-5335-48F8-A626-2D48166F0073}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" customWidth="1"/>
+    <col min="18" max="19" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="13.9">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,8 +760,14 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -797,8 +819,14 @@
       <c r="Q2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2">
+        <v>249.58</v>
+      </c>
+      <c r="S2">
+        <v>11.58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -850,8 +878,14 @@
       <c r="Q3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3">
+        <v>1019.53</v>
+      </c>
+      <c r="S3">
+        <v>3.7549999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -903,8 +937,14 @@
       <c r="Q4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4">
+        <v>1855.4</v>
+      </c>
+      <c r="S4">
+        <v>6.1050000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -956,8 +996,14 @@
       <c r="Q5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5">
+        <v>2102.13</v>
+      </c>
+      <c r="S5">
+        <v>12.855</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1009,8 +1055,14 @@
       <c r="Q6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6">
+        <v>209.5</v>
+      </c>
+      <c r="S6">
+        <v>7.9050000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1062,8 +1114,14 @@
       <c r="Q7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7">
+        <v>1816.17</v>
+      </c>
+      <c r="S7">
+        <v>3.0350000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1115,8 +1173,14 @@
       <c r="Q8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="S8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1168,8 +1232,14 @@
       <c r="Q9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9">
+        <v>0.22</v>
+      </c>
+      <c r="S9">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1221,8 +1291,14 @@
       <c r="Q10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10">
+        <v>0.24</v>
+      </c>
+      <c r="S10">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1274,8 +1350,14 @@
       <c r="Q11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11">
+        <v>0.26</v>
+      </c>
+      <c r="S11">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1327,8 +1409,14 @@
       <c r="Q12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12">
+        <v>339.73</v>
+      </c>
+      <c r="S12">
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1380,8 +1468,14 @@
       <c r="Q13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13">
+        <v>357.71</v>
+      </c>
+      <c r="S13">
+        <v>8.375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1433,8 +1527,14 @@
       <c r="Q14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14">
+        <v>1224.23</v>
+      </c>
+      <c r="S14">
+        <v>3.4950000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1486,8 +1586,14 @@
       <c r="Q15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15">
+        <v>1570.72</v>
+      </c>
+      <c r="S15">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1539,8 +1645,14 @@
       <c r="Q16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16">
+        <v>1558.8</v>
+      </c>
+      <c r="S16">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1591,6 +1703,12 @@
       </c>
       <c r="Q17" t="s">
         <v>22</v>
+      </c>
+      <c r="R17">
+        <v>769.38</v>
+      </c>
+      <c r="S17">
+        <v>136.38</v>
       </c>
     </row>
   </sheetData>
@@ -1601,20 +1719,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24E29A5-36F3-4B66-87D0-651F4F937DED}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1628,7 +1746,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1757,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1650,7 +1768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1661,7 +1779,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +1790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1801,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1812,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1705,7 +1823,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1716,7 +1834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1727,7 +1845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1738,7 +1856,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +1867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1763,7 +1881,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1774,7 +1892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1788,7 +1906,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1917,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1810,7 +1928,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1819,6 +1937,28 @@
       </c>
       <c r="C18" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>